<commit_message>
Add all benchmarking results
</commit_message>
<xml_diff>
--- a/tests/test_files/rutime_test_results/Results_Summary.xlsx
+++ b/tests/test_files/rutime_test_results/Results_Summary.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenzi\Documents\ASU_Courses\SER_401\PROJECT\TSK#274_Benchmark_Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenzi\Documents\ASU_Courses\SER_401\PROJECT\team-58\tests\test_files\rutime_test_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EC5F7C-3914-4681-9D9F-2C697F314650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C832C46F-3A14-4204-BB76-B7D8DD93D367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Single Process</t>
   </si>
@@ -59,24 +59,31 @@
     <t>300_Students</t>
   </si>
   <si>
-    <t>Runtime (Minutes)</t>
-  </si>
-  <si>
     <t>Runtime Improvement (Multi vs Single)</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>In Progress</t>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Midnight Constant</t>
+  </si>
+  <si>
+    <t>Runtimes (HH:MM:SS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="h:mm:ss.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -103,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -111,21 +118,183 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,114 +574,206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C031C810-20BA-4819-98D2-264C6F135EC6}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="1" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
-        <f>(44.12-27.62)/60</f>
-        <v>0.27499999999999997</v>
-      </c>
-      <c r="C3">
-        <f>(34.98-23.49)/60</f>
-        <v>0.19149999999999998</v>
-      </c>
-      <c r="D3" s="5">
-        <f>B3/C3 -1</f>
-        <v>0.43603133159268936</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="16">
+        <v>0.77184745370370367</v>
+      </c>
+      <c r="C4" s="17">
+        <v>0.77203842592592586</v>
+      </c>
+      <c r="D4" s="18">
+        <f>C4-B4</f>
+        <v>1.9097222222219656E-4</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.61346631944444441</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.61359930555555553</v>
+      </c>
+      <c r="G4" s="17">
+        <f>F4-E4</f>
+        <v>1.3298611111112191E-4</v>
+      </c>
+      <c r="H4" s="22">
+        <f>D4/G4 -1</f>
+        <v>0.43603133159237983</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
-        <f>59-36+(55.42-22.52)/60</f>
-        <v>23.548333333333332</v>
-      </c>
-      <c r="C4">
-        <f>60-52+(52.64-19.24)/60</f>
-        <v>8.5566666666666666</v>
-      </c>
-      <c r="D4" s="5">
-        <f>B4/C4-1</f>
-        <v>1.7520451889365014</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="16">
+        <v>0.77526064814814821</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.79161365740740741</v>
+      </c>
+      <c r="D5" s="18">
+        <f t="shared" ref="D5:D6" si="0">C5-B5</f>
+        <v>1.6353009259259199E-2</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.61966712962962966</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.62560925925925925</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" ref="G5:G7" si="1">F5-E5</f>
+        <v>5.9421296296295889E-3</v>
+      </c>
+      <c r="H5" s="22">
+        <f t="shared" ref="H5:H7" si="2">D5/G5 -1</f>
+        <v>1.7520451889365103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
-        <f>(34-33)+(15.51-29.49)/60</f>
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="C5">
-        <f>(37.56-9.83)/60</f>
-        <v>0.46216666666666673</v>
-      </c>
-      <c r="D5" s="5">
-        <f t="shared" ref="D4:D6" si="0">1-C5/B5</f>
-        <v>0.39743589743589736</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="16">
+        <v>0.77325798611111107</v>
+      </c>
+      <c r="C6" s="17">
+        <v>0.77379062500000007</v>
+      </c>
+      <c r="D6" s="18">
+        <f t="shared" si="0"/>
+        <v>5.3263888888899213E-4</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.61608599537037034</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.61640694444444444</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="1"/>
+        <v>3.2094907407409501E-4</v>
+      </c>
+      <c r="H6" s="22">
+        <f>D6/G6 -1</f>
+        <v>0.65957446808531972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <f>(18-15)*60+13+(60-45)+(39.48-18.18)/60</f>
-        <v>208.35499999999999</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
+      <c r="B7" s="19">
+        <v>0.87307488425925917</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.21499502314814814</v>
+      </c>
+      <c r="D7" s="21">
+        <f>A10-(B7-C7)</f>
+        <v>0.34192002314814829</v>
+      </c>
+      <c r="E7" s="19">
+        <v>0.65646041666666666</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0.75948472222222219</v>
+      </c>
+      <c r="G7" s="20">
+        <f t="shared" si="1"/>
+        <v>0.10302430555555553</v>
+      </c>
+      <c r="H7" s="23">
+        <f t="shared" si="2"/>
+        <v>2.3188287104130878</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.99999988425925934</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:D2"/>
+  <mergeCells count="4">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>